<commit_message>
Creating a commit to tag
</commit_message>
<xml_diff>
--- a/displayData.xlsx
+++ b/displayData.xlsx
@@ -7,29 +7,137 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="EmployeesList" sheetId="1" r:id="rId1"/>
+    <sheet name="October 2017" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+  <si>
+    <t>MonthlySalary</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>Total_Days_Worked</t>
+  </si>
+  <si>
+    <t>Advance_Balance</t>
+  </si>
+  <si>
+    <t>Advance_For_Month</t>
+  </si>
+  <si>
+    <t>Salary_For_Month</t>
+  </si>
   <si>
     <t>EmployeeName</t>
   </si>
   <si>
-    <t>Salary</t>
-  </si>
-  <si>
     <t>Shyamu</t>
+  </si>
+  <si>
+    <t>Ramu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -37,27 +145,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0000FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -72,11 +166,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,29 +462,349 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:AK3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="20" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+    <row r="1" spans="1:37">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:37">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>6000</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3">
+        <v>5000</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>